<commit_message>
Removed Hard core values, some changes in excel
</commit_message>
<xml_diff>
--- a/KeywordDriven/src/dataEngine/DataEngine.xlsx
+++ b/KeywordDriven/src/dataEngine/DataEngine.xlsx
@@ -4,29 +4,34 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="18960" windowHeight="8925" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="18960" windowHeight="8925"/>
   </bookViews>
   <sheets>
     <sheet name="TestSteps" sheetId="1" r:id="rId1"/>
     <sheet name="TestCases" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Settings" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="TS_001">TestSteps!$B$3:$B$6</definedName>
+    <definedName name="Action_Keyword">Settings!$D$2:$D$7</definedName>
+    <definedName name="Action_Keywords">Settings!$D$2:$D$7</definedName>
+    <definedName name="Login_Page">Settings!$B$2:$B$4</definedName>
+    <definedName name="Page_Name">Settings!$A$2:$A$3</definedName>
+    <definedName name="Startcentre_Page">Settings!$C$2</definedName>
+    <definedName name="TS_001">TestSteps!#REF!</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="48">
   <si>
     <t>TestCase ID</t>
   </si>
   <si>
-    <t>TS_ID</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -36,24 +41,6 @@
     <t>Login_01</t>
   </si>
   <si>
-    <t>TS_001</t>
-  </si>
-  <si>
-    <t>TS_002</t>
-  </si>
-  <si>
-    <t>TS_003</t>
-  </si>
-  <si>
-    <t>TS_004</t>
-  </si>
-  <si>
-    <t>TS_005</t>
-  </si>
-  <si>
-    <t>TS_006</t>
-  </si>
-  <si>
     <t>open the Browser</t>
   </si>
   <si>
@@ -66,21 +53,12 @@
     <t>navigate</t>
   </si>
   <si>
-    <t>Click on My account button on the Top Right Location</t>
-  </si>
-  <si>
-    <t>input_Username</t>
-  </si>
-  <si>
     <t>Enter the Password in Password field</t>
   </si>
   <si>
     <t>Enter the username in the Username Field</t>
   </si>
   <si>
-    <t>input_Password</t>
-  </si>
-  <si>
     <t>Click on Login button</t>
   </si>
   <si>
@@ -96,15 +74,6 @@
     <t>Close the Browser</t>
   </si>
   <si>
-    <t>TS_007</t>
-  </si>
-  <si>
-    <t>TS_008</t>
-  </si>
-  <si>
-    <t>TS_009</t>
-  </si>
-  <si>
     <t>Page Object</t>
   </si>
   <si>
@@ -114,9 +83,6 @@
     <t>closeBrowser</t>
   </si>
   <si>
-    <t>btn_MyAccount</t>
-  </si>
-  <si>
     <t>txtbx_Username</t>
   </si>
   <si>
@@ -132,36 +98,88 @@
     <t>Runmode</t>
   </si>
   <si>
-    <t>Login into the online store application</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>Purchase_02</t>
-  </si>
-  <si>
-    <t>Purchase a product</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
     <t>Results</t>
   </si>
   <si>
+    <t>Login into the maximo application</t>
+  </si>
+  <si>
+    <t>Step_02</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Test_Steps</t>
+  </si>
+  <si>
+    <t>Desc</t>
+  </si>
+  <si>
+    <t>Sno</t>
+  </si>
+  <si>
+    <t>Action keyword and page object should be dynamically picked from excel.</t>
+  </si>
+  <si>
+    <t>Read Excel once in to object and execute the test case instead reading line after line ( should declare object dynamically)</t>
+  </si>
+  <si>
+    <t>For every successfull step update Log file with (step num)  + pass/fail</t>
+  </si>
+  <si>
+    <t>In case of exception take screenshot and place it in exceptions filder and with subfolder name as testcase.
+  &gt;&gt; Exceptions &gt;&gt; LOGIN01 &gt;&gt;
+Also screenshot file name should be &lt;Date+timestamp&gt;_&lt;testcase step num&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make sure you skip any empty lines inbetween the test case </t>
+  </si>
+  <si>
+    <t>In case of exception in first test case ...you should jump to second testcase by leaving first one .</t>
+  </si>
+  <si>
+    <t>Data Set</t>
+  </si>
+  <si>
+    <t>maxadmin</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>Page Name</t>
+  </si>
+  <si>
+    <t>Login_Page</t>
+  </si>
+  <si>
+    <t>Startcentre_Page</t>
+  </si>
+  <si>
+    <t>Page_Name</t>
+  </si>
+  <si>
+    <t>Action_Keyword</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
     <t>PASS</t>
-  </si>
-  <si>
-    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,6 +195,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -187,18 +221,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -206,15 +240,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,194 +564,203 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="27.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" width="49.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="29.28515625" collapsed="true"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="42" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="27.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="29.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7" ht="15.75">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
       <c r="F2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>46</v>
+      </c>
+      <c r="G2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
       <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>39</v>
+      </c>
+      <c r="G4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
         <v>16</v>
       </c>
-      <c r="F5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="G6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
         <v>17</v>
       </c>
-      <c r="D6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" t="s">
-        <v>30</v>
+      <c r="G9" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C9">
+      <formula1>Page_Name</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E9">
+      <formula1>Action_Keyword</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D9">
+      <formula1>INDIRECT(D2)</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
@@ -706,54 +770,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="24.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="44.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="44" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>42</v>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -763,6 +827,281 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="32.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.5703125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75">
+      <c r="A1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="68.140625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="30">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="75">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="4"/>
+      <c r="B26" s="5"/>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="4"/>
+      <c r="B27" s="5"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="4"/>
+      <c r="B28" s="5"/>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="4"/>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="4"/>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="4"/>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="4"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="4"/>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="4"/>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>